<commit_message>
feat: Renamed Service Role mapping sheet name
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/ServiceRoleMapping_BBA9.xlsx
+++ b/src/functionalTest/resources/ServiceRoleMapping_BBA9.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:8001_{4393B2A3-4DAA-4A40-8C1D-282A4C5A9D5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F245E94-5576-F447-89EA-50B6CCAB5A54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19560" xr2:uid="{2E9A26E9-1D6D-094B-B75C-CEBE58038F70}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" xr2:uid="{2E9A26E9-1D6D-094B-B75C-CEBE58038F70}"/>
   </bookViews>
   <sheets>
-    <sheet name="IDAM Mapping" sheetId="1" r:id="rId1"/>
+    <sheet name="Service to CW Roles Mapping" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>

</xml_diff>

<commit_message>
RDCC-2278: feat: Modified tests to accomodate the new file changes
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/ServiceRoleMapping_BBA9.xlsx
+++ b/src/functionalTest/resources/ServiceRoleMapping_BBA9.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F245E94-5576-F447-89EA-50B6CCAB5A54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D1C4B0-452F-A24B-A903-ECC23F2D508A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" xr2:uid="{2E9A26E9-1D6D-094B-B75C-CEBE58038F70}"/>
   </bookViews>
   <sheets>
     <sheet name="Service to CW Roles Mapping" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,15 +42,9 @@
     <t>caseworker-iac</t>
   </si>
   <si>
-    <t>Roles</t>
-  </si>
-  <si>
     <t>Service ID</t>
   </si>
   <si>
-    <t>Idam Roles</t>
-  </si>
-  <si>
     <t>caseworker-iac-dwp</t>
   </si>
   <si>
@@ -58,6 +52,12 @@
   </si>
   <si>
     <t>caseworker-iac-bulkscan</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>IDAM Roles</t>
   </si>
 </sst>
 </file>
@@ -418,7 +418,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -429,13 +429,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -457,7 +457,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -468,7 +468,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -479,7 +479,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: RDCC-2278 Updated code to align with the Excel File structures (#147)
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/ServiceRoleMapping_BBA9.xlsx
+++ b/src/functionalTest/resources/ServiceRoleMapping_BBA9.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F245E94-5576-F447-89EA-50B6CCAB5A54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D1C4B0-452F-A24B-A903-ECC23F2D508A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" xr2:uid="{2E9A26E9-1D6D-094B-B75C-CEBE58038F70}"/>
   </bookViews>
   <sheets>
     <sheet name="Service to CW Roles Mapping" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,15 +42,9 @@
     <t>caseworker-iac</t>
   </si>
   <si>
-    <t>Roles</t>
-  </si>
-  <si>
     <t>Service ID</t>
   </si>
   <si>
-    <t>Idam Roles</t>
-  </si>
-  <si>
     <t>caseworker-iac-dwp</t>
   </si>
   <si>
@@ -58,6 +52,12 @@
   </si>
   <si>
     <t>caseworker-iac-bulkscan</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>IDAM Roles</t>
   </si>
 </sst>
 </file>
@@ -418,7 +418,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -429,13 +429,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -457,7 +457,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -468,7 +468,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -479,7 +479,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RDCC-5182 Added Version check
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/ServiceRoleMapping_BBA9.xlsx
+++ b/src/functionalTest/resources/ServiceRoleMapping_BBA9.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/functionalTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_2088737/IdeaProjects/refdata_workspace/RDCC-5182/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D1C4B0-452F-A24B-A903-ECC23F2D508A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4BB7A4-5AE8-D848-89C1-14C151A3786E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" xr2:uid="{2E9A26E9-1D6D-094B-B75C-CEBE58038F70}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19520" activeTab="1" xr2:uid="{2E9A26E9-1D6D-094B-B75C-CEBE58038F70}"/>
   </bookViews>
   <sheets>
     <sheet name="Service to CW Roles Mapping" sheetId="1" r:id="rId1"/>
+    <sheet name="VERSION" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>BBA9</t>
   </si>
@@ -58,6 +59,12 @@
   </si>
   <si>
     <t>IDAM Roles</t>
+  </si>
+  <si>
+    <t>File version</t>
+  </si>
+  <si>
+    <t>vx.xx</t>
   </si>
 </sst>
 </file>
@@ -417,7 +424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72EC9574-42D9-2D49-9FE6-FC22AA6AFF8E}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -486,4 +493,27 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6322A88E-3B13-2E4E-AB8E-32BED887BA98}">
+  <dimension ref="A6:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
RDCC-5182 fixed the review comments
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/ServiceRoleMapping_BBA9.xlsx
+++ b/src/functionalTest/resources/ServiceRoleMapping_BBA9.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_2088737/IdeaProjects/refdata_workspace/RDCC-5182/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4BB7A4-5AE8-D848-89C1-14C151A3786E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513F04BB-F919-6446-9BCD-04F129EF43FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19520" activeTab="1" xr2:uid="{2E9A26E9-1D6D-094B-B75C-CEBE58038F70}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19520" xr2:uid="{2E9A26E9-1D6D-094B-B75C-CEBE58038F70}"/>
   </bookViews>
   <sheets>
     <sheet name="Service to CW Roles Mapping" sheetId="1" r:id="rId1"/>
-    <sheet name="VERSION" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>BBA9</t>
   </si>
@@ -59,12 +58,6 @@
   </si>
   <si>
     <t>IDAM Roles</t>
-  </si>
-  <si>
-    <t>File version</t>
-  </si>
-  <si>
-    <t>vx.xx</t>
   </si>
 </sst>
 </file>
@@ -424,7 +417,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72EC9574-42D9-2D49-9FE6-FC22AA6AFF8E}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -493,27 +486,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6322A88E-3B13-2E4E-AB8E-32BED887BA98}">
-  <dimension ref="A6:B6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Replace iac roles (#744)
* Replace iac roles

* Replace iac roles

* Replace iac roles

* Replace iac roles

* Replace iac roles

* Replace iac roles

* SUPPRESS CVE
</commit_message>
<xml_diff>
--- a/src/functionalTest/resources/ServiceRoleMapping_BBA9.xlsx
+++ b/src/functionalTest/resources/ServiceRoleMapping_BBA9.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_224557/Documents/GitHub/duplicate/rd-caseworker-ref-api/src/functionalTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_sahitya/Documents/GitRepos/rd-caseworker-ref-api/src/functionalTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D1C4B0-452F-A24B-A903-ECC23F2D508A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C4F4C9-2BA6-7A44-A97A-B95622D9FBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19520" xr2:uid="{2E9A26E9-1D6D-094B-B75C-CEBE58038F70}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30720" windowHeight="17820" xr2:uid="{2E9A26E9-1D6D-094B-B75C-CEBE58038F70}"/>
   </bookViews>
   <sheets>
     <sheet name="Service to CW Roles Mapping" sheetId="1" r:id="rId1"/>
@@ -36,28 +36,28 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
-    <t>BBA9</t>
-  </si>
-  <si>
-    <t>caseworker-iac</t>
-  </si>
-  <si>
     <t>Service ID</t>
   </si>
   <si>
-    <t>caseworker-iac-dwp</t>
-  </si>
-  <si>
-    <t>caseworker-senior-iac</t>
-  </si>
-  <si>
-    <t>caseworker-iac-bulkscan</t>
-  </si>
-  <si>
     <t>Role</t>
   </si>
   <si>
     <t>IDAM Roles</t>
+  </si>
+  <si>
+    <t>caseworker-ia</t>
+  </si>
+  <si>
+    <t>caseworker-ia-caseofficer</t>
+  </si>
+  <si>
+    <t>caseworker-civil</t>
+  </si>
+  <si>
+    <t>caseworker-civil-staff</t>
+  </si>
+  <si>
+    <t>BFA1</t>
   </si>
 </sst>
 </file>
@@ -418,7 +418,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -429,57 +429,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>